<commit_message>
Update PC Value Tracker documentation and monthly report generation
</commit_message>
<xml_diff>
--- a/PC_Value_Tracker/output/monthly/Monthly_Report_2026-01.xlsx
+++ b/PC_Value_Tracker/output/monthly/Monthly_Report_2026-01.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-01-25 07:04</t>
+          <t>2026-01-27 07:17</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -512,251 +512,311 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Project</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Diagnostic</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>BY SYSTEM</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Alarm</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>DCS</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>DCS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Network</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PLC</t>
+          <t>Alarm</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HMI</t>
+          <t>SIS</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>BY COMPLEXITY</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PLC</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>HMI</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Quick</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>7</v>
-      </c>
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>6</v>
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>BY COMPLEXITY</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>BY BUSINESS IMPACT</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>BY BUSINESS IMPACT</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>Compliance</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Safety</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Efficiency</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr"/>
-      <c r="B30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>BY RESOLUTION</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
+      <c r="B31" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Efficiency</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Production</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>BY RESOLUTION</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Informational</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>Handed Off</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B40" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+    <row r="41">
+      <c r="A41" t="inlineStr">
         <is>
           <t>Escalated</t>
         </is>
       </c>
-      <c r="B35" t="n">
-        <v>1</v>
+      <c r="B41" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -770,7 +830,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -818,37 +878,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DCS — Experion</t>
+          <t>DCS: Experion, C300</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Auto-suppress 57DAS002 recommendation.</t>
+          <t>Documented New Year’s ETD leak impact; restored multiple IOMs/FTAs and returned controls to Ops.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Handed Off</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Production</t>
         </is>
       </c>
     </row>
@@ -860,12 +920,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Alarm: DynAMo</t>
+          <t>DCS — Experion</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Advised adding self-suppression on trigger tag 57DAS002</t>
+          <t>Auto-suppress 57DAS002 recommendation.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -880,7 +940,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Handed Off</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -897,22 +957,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>DCS: Experion, C300</t>
+          <t>Alarm: DynAMo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Coordinated data request on Event Archive and C300 checkpoints</t>
+          <t>Advised adding self-suppression on trigger tag 57DAS002</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Applications</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Quick</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -934,17 +994,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Integrity</t>
+          <t>DCS: Experion, C300</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Identified 48k missing Alarm Group defects in Integrity</t>
+          <t>Coordinated data request on Event Archive and C300 checkpoints</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -959,24 +1019,24 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Alarm: ACM</t>
+          <t>Integrity</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Escalated missing 1Crude alarm tags after server move</t>
+          <t>Identified 48k missing Alarm Group defects in Integrity</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -996,24 +1056,24 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Network: FTE</t>
+          <t>DCS: Experion, C300</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Asked about migration need for Experion Network Manager R102</t>
+          <t>Provided Wilmington C300 checkpoint snapshot and Honeywell audit reference; recommended standardizing checkpoint/event archive settings across controllers.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1023,44 +1083,44 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Efficiency</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Alarm — DynAMo</t>
+          <t>SIS: Triconex / IPF logic</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Collection alert (LARRS430); SHB failover; no data after.</t>
+          <t>Sent prioritized list of HGU IPF alarms to investigate.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Diagnostic</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1070,24 +1130,24 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Safety</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Integrity — PAS Integrity</t>
+          <t>Alarm: ACM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FTP timing race on cfirsthop before Integrity read.</t>
+          <t>Escalated missing 1Crude alarm tags after server move</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1097,7 +1157,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1107,34 +1167,34 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Alarm Flood</t>
+          <t>SIS: Triconex</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Alarm flood KPI analysis</t>
+          <t>Cleared fan-run first-out during hardware work; flagged logic change that will require MOC to prevent recurrence.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Project</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1144,24 +1204,24 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Safety</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DCS — Experion</t>
+          <t>Network: FTE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ISOM OPCI channel Marginal; ACE reload (ACT → CEE).</t>
+          <t>Asked about migration need for Experion Network Manager R102</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1171,49 +1231,49 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Quick</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Network: OPC</t>
+          <t>Integrity: Change management</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Mapped 42 HDA/DA configs restoring Integrity connectivity</t>
+          <t>Shared PMOC form for software change; noted applicability of steps for first deployment on live unit.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Project</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Quick</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1225,22 +1285,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Integrity</t>
+          <t>Other (facility monitoring)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Reported missing Triconex detail, raised MOC concern</t>
+          <t>Proposed temporary water leak detector tied to console alarms for ETD rack room until roof repair is verified.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1255,76 +1315,76 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Efficiency</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Alarm — ACM</t>
+          <t>Other (facility remediation)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Restored missing tags 38L331N/38L330N; TagSync review.</t>
+          <t>Requested Facilities address recurring ETD roof leaks; asked for plan/timeline.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Diagnostic</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Efficiency</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DCS — Experion (EPKS)</t>
+          <t>Alarm — DynAMo</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Controller hardware info remediation confirmed.</t>
+          <t>Collection alert (LARRS430); SHB failover; no data after.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Applications</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1336,54 +1396,54 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Alarm — DynAMo</t>
+          <t>SIS: Trident</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>DL creation for UTIL DynAMo reports; verification offered.</t>
+          <t>Reported CRU console IPF DI module fault; cleared via EDM; will monitor.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Safety</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Historian — SQL</t>
+          <t>SIS: Trident / Vendor case</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Deleted LAREventsrepl during cHISTSQL2 cleanup.</t>
+          <t>Shared DO 3626X fault evidence; provided EDM screenshots to Schneider; awaiting guidance.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1393,39 +1453,39 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Handed Off</t>
+          <t>Escalated</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Safety</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Integrity — PAS Integrity</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Analyzed backup utility Relocate Files step during troubleshooting</t>
+          <t>FTP timing race on cfirsthop before Integrity read.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Applications</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1440,24 +1500,24 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PLC — ControlEdge / UOC</t>
+          <t>Alarm Flood</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Enabled commissioning; staged ControlEdge Builder installers.</t>
+          <t>Alarm flood KPI analysis</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1467,7 +1527,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1477,98 +1537,98 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>HMI — Experion HS</t>
+          <t>DCS: Experion (RIO/IO Link)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Panel PC install error; missing Panel Server license.</t>
+          <t>Coordinated and confirmed Water Well #18 &amp; Sub 8 RIO IO-Link cutovers; Ops verified control restored.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Project</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Production</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Alarm — HAM</t>
+          <t>APC: Blending (PBO)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>HAM 2.2→2.3 upgrade license follow-up and escalation.</t>
+          <t>Shared experience that PBO server restart resolved indicator issues.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Applications</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Quick</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Escalated</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Efficiency</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>HMI: HMIWeb</t>
+          <t>DCS — Experion</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Responded to Panel PC install error missing Panel Server option</t>
+          <t>ISOM OPCI channel Marginal; ACE reload (ACT → CEE).</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1578,12 +1638,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1595,37 +1655,740 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Network: OPC</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Mapped 42 HDA/DA configs restoring Integrity connectivity</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Integrity</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Reported missing Triconex detail, raised MOC concern</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DCS: Experion (hardware)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Replaced HTU4 DCS power supply with Trey; cleared alarm and restored normal state.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>DCS: Experion (DO relay card)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Replaced DO relay card for ETD TK-158 timer valve; observed significant corrosion indicating late failure; unit back healthy.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SIS: Safety Manager</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Advised on Safety Builder memory error; pointed to timerbase memory usage.</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Informational</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Alarm — ACM</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Restored missing tags 38L331N/38L330N; TagSync review.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>DCS — Experion (EPKS)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Controller hardware info remediation confirmed.</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Alarm — DynAMo</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>DL creation for UTIL DynAMo reports; verification offered.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Historian — SQL</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Deleted LAREventsrepl during cHISTSQL2 cleanup.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Handed Off</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SIS: Trident</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Cleared DI module fault in Trident via EDM; no recurrence after a week; closed item.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Analyzed backup utility Relocate Files step during troubleshooting</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Efficiency</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Alarm: Asset Intellect/DynAMo</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Explained 13FY2000 alarm under asset; suggested cleanup plan.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Informational</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>2026-01-22</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>PLC — ControlEdge / UOC</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Enabled commissioning; staged ControlEdge Builder installers.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>HMI — Experion HS</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Panel PC install error; missing Panel Server license.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Alarm — HAM</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>HAM 2.2→2.3 upgrade license follow-up and escalation.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Escalated</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>HMI: HMIWeb</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Responded to Panel PC install error missing Panel Server option</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>PLC: ControlEdge</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>Staged latest ControlEdge Builder media for commissioning</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>Day-to-Day</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Low</t>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>DCS: Experion, C300</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Investigated unexpected SP change on 3PC5140; traced to OP failure and module switchover; Instrument repaired water intrusion in valve positioner; SP stable; closed task.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Integrity: I/O reservations</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Issued AMP I/O reservation (ARF) for LAR6W existing points in 41-C300-1.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Project</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Informational</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Network: Experion/ETD access</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Troubleshot failed logins from ETD to clusters; removed ETD subscriptions and asked to confirm; planning TAC case.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Efficiency</t>
         </is>
       </c>
     </row>
@@ -1640,7 +2403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1887,32 +2650,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Network: OPC</t>
+          <t>APC: Blending (PBO)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Mapped 42 HDA/DA configs restoring Integrity connectivity</t>
+          <t>Shared experience that PBO server restart resolved indicator issues.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Quick</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Efficiency</t>
         </is>
       </c>
     </row>
@@ -1924,261 +2687,261 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Integrity</t>
+          <t>Network: OPC</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Reported missing Triconex detail, raised MOC concern</t>
+          <t>Mapped 42 HDA/DA configs restoring Integrity connectivity</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Alarm — ACM</t>
+          <t>Integrity</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Restored missing tags 38L331N/38L330N; TagSync review.</t>
+          <t>Reported missing Triconex detail, raised MOC concern</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SIS: Safety Manager</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Advised on Safety Builder memory error; pointed to timerbase memory usage.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Informational</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>2026-01-20</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Alarm — DynAMo</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>DL creation for UTIL DynAMo reports; verification offered.</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Alarm — ACM</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Restored missing tags 38L331N/38L330N; TagSync review.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> === DAY-TO-DAY ===</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Alarm — DynAMo</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>DL creation for UTIL DynAMo reports; verification offered.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>System</t>
+          <t>Alarm: Asset Intellect/DynAMo</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Summary</t>
+          <t>Explained 13FY2000 alarm under asset; suggested cleanup plan.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Complexity</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Resolution</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Impact</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2026-01-06</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>DCS: Experion, C300</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Coordinated data request on Event Archive and C300 checkpoints</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Network: FTE</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Asked about migration need for Experion Network Manager R102</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Quick</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Compliance</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> === DAY-TO-DAY ===</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Alarm Flood</t>
+          <t>System</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Alarm flood KPI analysis</t>
+          <t>Summary</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Complexity</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Resolution</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Compliance</t>
+          <t>Impact</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DCS — Experion</t>
+          <t>DCS: Experion, C300</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ISOM OPCI channel Marginal; ACE reload (ACT → CEE).</t>
+          <t>Documented New Year’s ETD leak impact; restored multiple IOMs/FTAs and returned controls to Ops.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>High</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2188,34 +2951,34 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Production</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DCS — Experion (EPKS)</t>
+          <t>DCS: Experion, C300</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Controller hardware info remediation confirmed.</t>
+          <t>Coordinated data request on Event Archive and C300 checkpoints</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2227,54 +2990,54 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Historian — SQL</t>
+          <t>DCS: Experion, C300</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Deleted LAREventsrepl during cHISTSQL2 cleanup.</t>
+          <t>Provided Wilmington C300 checkpoint snapshot and Honeywell audit reference; recommended standardizin</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Handed Off</t>
+          <t>Informational</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Efficiency</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Network: FTE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Analyzed backup utility Relocate Files step during troubleshooting</t>
+          <t>Asked about migration need for Experion Network Manager R102</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Quick</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2284,29 +3047,29 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Efficiency</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>PLC — ControlEdge / UOC</t>
+          <t>Other (facility monitoring)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Enabled commissioning; staged ControlEdge Builder installers.</t>
+          <t>Proposed temporary water leak detector tied to console alarms for ETD rack room until roof repair is</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2316,61 +3079,61 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Efficiency</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>HMI — Experion HS</t>
+          <t>SIS: Trident</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Panel PC install error; missing Panel Server license.</t>
+          <t>Reported CRU console IPF DI module fault; cleared via EDM; will monitor.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Fixed</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Safety</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Alarm — HAM</t>
+          <t>SIS: Trident / Vendor case</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>HAM 2.2→2.3 upgrade license follow-up and escalation.</t>
+          <t>Shared DO 3626X fault evidence; provided EDM screenshots to Schneider; awaiting guidance.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2380,29 +3143,29 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Safety</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>HMI: HMIWeb</t>
+          <t>Alarm Flood</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Responded to Panel PC install error missing Panel Server option</t>
+          <t>Alarm flood KPI analysis</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2412,49 +3175,761 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Compliance</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>DCS — Experion</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ISOM OPCI channel Marginal; ACE reload (ACT → CEE).</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>DCS: Experion (hardware)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Replaced HTU4 DCS power supply with Trey; cleared alarm and restored normal state.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>DCS: Experion (DO relay card)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Replaced DO relay card for ETD TK-158 timer valve; observed significant corrosion indicating late fa</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>DCS — Experion (EPKS)</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Controller hardware info remediation confirmed.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Historian — SQL</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Deleted LAREventsrepl during cHISTSQL2 cleanup.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Handed Off</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SIS: Trident</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Cleared DI module fault in Trident via EDM; no recurrence after a week; closed item.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Analyzed backup utility Relocate Files step during troubleshooting</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Efficiency</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>2026-01-22</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>PLC — ControlEdge / UOC</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Enabled commissioning; staged ControlEdge Builder installers.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>HMI — Experion HS</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Panel PC install error; missing Panel Server license.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Alarm — HAM</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>HAM 2.2→2.3 upgrade license follow-up and escalation.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Escalated</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>HMI: HMIWeb</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Responded to Panel PC install error missing Panel Server option</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>PLC: ControlEdge</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>Staged latest ControlEdge Builder media for commissioning</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>DCS: Experion, C300</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Investigated unexpected SP change on 3PC5140; traced to OP failure and module switchover; Instrument</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Network: Experion/ETD access</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Troubleshot failed logins from ETD to clusters; removed ETD subscriptions and asked to confirm; plan</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Efficiency</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> === DIAGNOSTIC ===</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Complexity</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Resolution</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Impact</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SIS: Triconex / IPF logic</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Sent prioritized list of HGU IPF alarms to investigate.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Other (facility remediation)</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Requested Facilities address recurring ETD roof leaks; asked for plan/timeline.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Efficiency</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> === PROJECT ===</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Complexity</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Resolution</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Impact</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SIS: Triconex</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Cleared fan-run first-out during hardware work; flagged logic change that will require MOC to preven</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Integrity: Change management</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Shared PMOC form for software change; noted applicability of steps for first deployment on live unit</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Informational</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>DCS: Experion (RIO/IO Link)</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Coordinated and confirmed Water Well #18 &amp; Sub 8 RIO IO-Link cutovers; Ops verified control restored</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Integrity: I/O reservations</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Issued AMP I/O reservation (ARF) for LAR6W existing points in 41-C300-1.</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Informational</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2467,7 +3942,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2678,43 +4153,59 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Alarm: Asset Intellect/DynAMo</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Explained 13FY2000 alarm under asset; suggested cleanup plan.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>2026-01-22</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Alarm — HAM</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>HAM 2.2→2.3 upgrade license follow-up and escalation.</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Day-to-Day</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Moderate</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-    </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> === DCS ===</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -2723,61 +4214,45 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Summary</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Stream</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Complexity</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> === DCS ===</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DCS — Experion</t>
+          <t>System</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Auto-suppress 57DAS002 recommendation.</t>
+          <t>Summary</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Stream</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Complexity</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2787,7 +4262,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Coordinated data request on Event Archive and C300 checkpoints</t>
+          <t>Documented New Year’s ETD leak impact; restored multiple IOMs/FTAs and returned controls to Ops.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2797,14 +4272,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2814,34 +4289,34 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ISOM OPCI channel Marginal; ACE reload (ACT → CEE).</t>
+          <t>Auto-suppress 57DAS002 recommendation.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Applications</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Quick</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DCS — Experion (EPKS)</t>
+          <t>DCS: Experion, C300</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Controller hardware info remediation confirmed.</t>
+          <t>Coordinated data request on Event Archive and C300 checkpoints</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2851,24 +4326,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>HMI — Experion HS</t>
+          <t>DCS: Experion, C300</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Panel PC install error; missing Panel Server license.</t>
+          <t>Provided Wilmington C300 checkpoint snapshot and Honeywell audit reference; recommended standardizin</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2878,69 +4353,105 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DCS: Experion (RIO/IO Link)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Coordinated and confirmed Water Well #18 &amp; Sub 8 RIO IO-Link cutovers; Ops verified control restored</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Project</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> === NETWORK ===</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DCS — Experion</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ISOM OPCI channel Marginal; ACE reload (ACT → CEE).</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>System</t>
+          <t>DCS: Experion (hardware)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Summary</t>
+          <t>Replaced HTU4 DCS power supply with Trey; cleared alarm and restored normal state.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Stream</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Complexity</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Network: FTE</t>
+          <t>DCS: Experion (DO relay card)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Asked about migration need for Experion Network Manager R102</t>
+          <t>Replaced DO relay card for ETD TK-158 timer valve; observed significant corrosion indicating late fa</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2950,177 +4461,177 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Quick</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Network: OPC</t>
+          <t>DCS — Experion (EPKS)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Mapped 42 HDA/DA configs restoring Integrity connectivity</t>
+          <t>Controller hardware info remediation confirmed.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Quick</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>HMI — Experion HS</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Panel PC install error; missing Panel Server license.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> === OTHER ===</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>DCS: Experion, C300</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Investigated unexpected SP change on 3PC5140; traced to OP failure and module switchover; Instrument</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>System</t>
+          <t>Network: Experion/ETD access</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Summary</t>
+          <t>Troubleshot failed logins from ETD to clusters; removed ETD subscriptions and asked to confirm; plan</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Stream</t>
+          <t>Day-to-Day</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Complexity</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2026-01-06</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Integrity</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Identified 48k missing Alarm Group defects in Integrity</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Applications</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Integrity — PAS Integrity</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>FTP timing race on cfirsthop before Integrity read.</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Applications</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> === NETWORK ===</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Integrity</t>
+          <t>System</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Reported missing Triconex detail, raised MOC concern</t>
+          <t>Summary</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Applications</t>
+          <t>Stream</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Complexity</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Historian — SQL</t>
+          <t>Network: FTE</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Deleted LAREventsrepl during cHISTSQL2 cleanup.</t>
+          <t>Asked about migration need for Experion Network Manager R102</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -3137,59 +4648,43 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Network: OPC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Analyzed backup utility Relocate Files step during troubleshooting</t>
+          <t>Mapped 42 HDA/DA configs restoring Integrity connectivity</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Applications</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Moderate</t>
+          <t>Medium</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2026-01-22</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>HMI: HMIWeb</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Responded to Panel PC install error missing Panel Server option</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Day-to-Day</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> === OTHER ===</t>
+        </is>
+      </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
@@ -3198,60 +4693,76 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> === PLC ===</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Stream</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Complexity</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>System</t>
+          <t>Integrity</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Summary</t>
+          <t>Identified 48k missing Alarm Group defects in Integrity</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Stream</t>
+          <t>Applications</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Complexity</t>
+          <t>Low</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>PLC — ControlEdge / UOC</t>
+          <t>Integrity: Change management</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Enabled commissioning; staged ControlEdge Builder installers.</t>
+          <t>Shared PMOC form for software change; noted applicability of steps for first deployment on live unit</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Day-to-Day</t>
+          <t>Project</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -3263,36 +4774,558 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Other (facility monitoring)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Proposed temporary water leak detector tied to console alarms for ETD rack room until roof repair is</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Other (facility remediation)</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Requested Facilities address recurring ETD roof leaks; asked for plan/timeline.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Diagnostic</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Integrity — PAS Integrity</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>FTP timing race on cfirsthop before Integrity read.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-15</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>APC: Blending (PBO)</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Shared experience that PBO server restart resolved indicator issues.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Integrity</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Reported missing Triconex detail, raised MOC concern</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Historian — SQL</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Deleted LAREventsrepl during cHISTSQL2 cleanup.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Analyzed backup utility Relocate Files step during troubleshooting</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>2026-01-22</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>HMI: HMIWeb</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Responded to Panel PC install error missing Panel Server option</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Integrity: I/O reservations</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Issued AMP I/O reservation (ARF) for LAR6W existing points in 41-C300-1.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Project</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> === PLC ===</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Stream</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Complexity</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PLC — ControlEdge / UOC</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Enabled commissioning; staged ControlEdge Builder installers.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>PLC: ControlEdge</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>Staged latest ControlEdge Builder media for commissioning</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>Day-to-Day</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr"/>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> === SIS ===</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Stream</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Complexity</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SIS: Triconex / IPF logic</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Sent prioritized list of HGU IPF alarms to investigate.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Diagnostic</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SIS: Triconex</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Cleared fan-run first-out during hardware work; flagged logic change that will require MOC to preven</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Project</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SIS: Trident</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Reported CRU console IPF DI module fault; cleared via EDM; will monitor.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>SIS: Trident / Vendor case</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Shared DO 3626X fault evidence; provided EDM screenshots to Schneider; awaiting guidance.</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2026-01-19</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SIS: Safety Manager</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Advised on Safety Builder memory error; pointed to timerbase memory usage.</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Applications</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-01-20</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SIS: Trident</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Cleared DI module fault in Trident via EDM; no recurrence after a week; closed item.</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Day-to-Day</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>